<commit_message>
update readme and summary
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenhao/Documents/Research/Empirical Study of Unit Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenhao/Documents/Research/Empirical-Study-of-Unit-Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D078F1-B373-CA47-974C-58AA47CD3405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD4A517-B56C-6E49-8099-F219406AC975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="-24260" windowWidth="28240" windowHeight="16260" xr2:uid="{09DD74C9-000B-C147-A52E-FA382DA941DB}"/>
+    <workbookView xWindow="260" yWindow="540" windowWidth="28240" windowHeight="16260" xr2:uid="{09DD74C9-000B-C147-A52E-FA382DA941DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +183,31 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -215,7 +240,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -225,16 +250,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -555,7 +589,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -581,7 +615,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -590,19 +624,19 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
@@ -614,7 +648,7 @@
       <c r="C4">
         <v>12</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -628,7 +662,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -642,21 +676,21 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" s="8" customFormat="1">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -670,12 +704,12 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -684,42 +718,42 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="3"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="3"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="3"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C12">
         <v>23</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f>SUM(C2:C12)</f>
         <v>63</v>
       </c>

</xml_diff>